<commit_message>
1.1 - Registro de Auditoria e Senhas
Adicionada a função de registro de auditoria, que guarda a maior parte das atividades no site. Também houveram alterações em como senhas funcionam: os usuários definem suas próprias senhas na primeira vez que fizerem login, e o administrador pode apagar a senha deles para redefiní-las caso seja necessário.
</commit_message>
<xml_diff>
--- a/assets/sheet_model.xlsx
+++ b/assets/sheet_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\T1DEV-T2\ArturV\Programas\Pessoal\projeto_instrumentacao\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artur\Documents\Tuta\dev\Python\projeto_instrumentacao\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9ED0C9-D1CF-4FBB-B50A-978A1009CE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DE5A9-3157-4628-96FD-B5150C89B3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuários" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>NOME</t>
   </si>
@@ -39,16 +39,10 @@
     <t>ADMIN</t>
   </si>
   <si>
-    <t>SENHA</t>
-  </si>
-  <si>
     <t>Exemplo</t>
   </si>
   <si>
-    <t>exemplo@exemplo.com</t>
-  </si>
-  <si>
-    <t>senha1234</t>
+    <t>exemplo@exemplo</t>
   </si>
 </sst>
 </file>
@@ -80,7 +74,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,8 +87,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,12 +102,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -120,6 +135,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -421,18 +440,18 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -443,33 +462,29 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>12345678910</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>12345678909</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
     </row>
   </sheetData>

</xml_diff>